<commit_message>
added a new endpoint
</commit_message>
<xml_diff>
--- a/adcomsys.xlsx
+++ b/adcomsys.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Flutter Fiesta" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Widsom War" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Coders Brawl" state="visible" r:id="rId6"/>
-    <sheet sheetId="4" name="Poster Compedition" state="visible" r:id="rId7"/>
+    <sheet sheetId="1" name="FLUTTER FIESTA" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="WISDOM WAR" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="CODERS BRAWL" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="POSTER COMPEDITION" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="28">
   <si>
     <t>MobileNumber</t>
   </si>
@@ -58,34 +58,46 @@
     <t>7044522841</t>
   </si>
   <si>
+    <t>Santadip Rudra</t>
+  </si>
+  <si>
+    <t>dipakrudra8@gmail.com</t>
+  </si>
+  <si>
+    <t>Wisdom War</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Great</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Flutter Fiesta</t>
+  </si>
+  <si>
+    <t>Coders Brawl</t>
+  </si>
+  <si>
     <t>Dipak Rudra</t>
   </si>
   <si>
-    <t>dipakrudra8@gmail.com</t>
-  </si>
-  <si>
-    <t>Flutter Fiesta</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Great</t>
-  </si>
-  <si>
-    <t>5</t>
+    <t>Poster Compedition</t>
   </si>
 </sst>
 </file>
@@ -462,6 +474,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="3" width="50" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="13" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
@@ -529,10 +681,10 @@
         <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
@@ -559,9 +711,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -611,15 +763,138 @@
         <v>12</v>
       </c>
     </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -669,62 +944,250 @@
         <v>12</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="13" width="10" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>